<commit_message>
Se realizan cambios para sanity semilla 10
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -222,12 +222,6 @@
     <t>732111324707275</t>
   </si>
   <si>
-    <t>3045984642</t>
-  </si>
-  <si>
-    <t>732111193278730</t>
-  </si>
-  <si>
     <t>81670</t>
   </si>
   <si>
@@ -304,6 +298,12 @@
   </si>
   <si>
     <t>936620047</t>
+  </si>
+  <si>
+    <t>3045981670</t>
+  </si>
+  <si>
+    <t>732111193278811</t>
   </si>
 </sst>
 </file>
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -952,7 +952,8 @@
     <col min="2" max="2" width="24.26953125" customWidth="1"/>
     <col min="3" max="3" width="30.1796875" customWidth="1"/>
     <col min="4" max="4" width="28.1796875" customWidth="1"/>
-    <col min="5" max="5" width="35.81640625" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
@@ -986,13 +987,13 @@
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -1026,10 +1027,10 @@
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
@@ -1049,19 +1050,19 @@
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>50</v>
@@ -1072,24 +1073,24 @@
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>23</v>
@@ -1132,7 +1133,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>56</v>
@@ -1141,7 +1142,7 @@
         <v>57</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>59</v>
@@ -1161,7 +1162,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>63</v>
@@ -1170,19 +1171,19 @@
         <v>64</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1">
@@ -1190,7 +1191,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>56</v>
@@ -1204,13 +1205,13 @@
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1">
@@ -1218,13 +1219,13 @@
         <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1232,13 +1233,13 @@
         <v>31</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se ajustan botones de entrada de mercancia e inventario
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla10\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\SanitySemillas\SanitySemilla10\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA1763B-52AB-4F86-8372-74F8BE5902A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="100">
   <si>
     <t>MSIDN</t>
   </si>
@@ -195,15 +196,6 @@
     <t>portId</t>
   </si>
   <si>
-    <t>3043208091</t>
-  </si>
-  <si>
-    <t>732111324707274</t>
-  </si>
-  <si>
-    <t>3045981684</t>
-  </si>
-  <si>
     <t>732111193278813</t>
   </si>
   <si>
@@ -216,12 +208,6 @@
     <t>00002201108240181684</t>
   </si>
   <si>
-    <t>3043209773</t>
-  </si>
-  <si>
-    <t>732111324707275</t>
-  </si>
-  <si>
     <t>81670</t>
   </si>
   <si>
@@ -234,18 +220,6 @@
     <t>3043209819</t>
   </si>
   <si>
-    <t>732111324707276</t>
-  </si>
-  <si>
-    <t>732111324707277</t>
-  </si>
-  <si>
-    <t>732111324707278</t>
-  </si>
-  <si>
-    <t>3043209863</t>
-  </si>
-  <si>
     <t>3043209868</t>
   </si>
   <si>
@@ -282,34 +256,82 @@
     <t>siebel05</t>
   </si>
   <si>
-    <t>470947400</t>
-  </si>
-  <si>
-    <t>675130993</t>
-  </si>
-  <si>
-    <t>426038582</t>
-  </si>
-  <si>
-    <t>17439454</t>
-  </si>
-  <si>
-    <t>1078584391</t>
-  </si>
-  <si>
-    <t>936620047</t>
-  </si>
-  <si>
-    <t>3045981670</t>
-  </si>
-  <si>
     <t>732111193278811</t>
+  </si>
+  <si>
+    <t>3046010569</t>
+  </si>
+  <si>
+    <t>732111193280551</t>
+  </si>
+  <si>
+    <t>732111193280535</t>
+  </si>
+  <si>
+    <t>399840300</t>
+  </si>
+  <si>
+    <t>592168140</t>
+  </si>
+  <si>
+    <t>313778543</t>
+  </si>
+  <si>
+    <t>994114856</t>
+  </si>
+  <si>
+    <t>721106626</t>
+  </si>
+  <si>
+    <t>3052754289</t>
+  </si>
+  <si>
+    <t>3052754293</t>
+  </si>
+  <si>
+    <t>3052754321</t>
+  </si>
+  <si>
+    <t>3046008586</t>
+  </si>
+  <si>
+    <t>3046008587</t>
+  </si>
+  <si>
+    <t>732111324709674</t>
+  </si>
+  <si>
+    <t>732111324709675</t>
+  </si>
+  <si>
+    <t>732111324709676</t>
+  </si>
+  <si>
+    <t>732111193278871</t>
+  </si>
+  <si>
+    <t>732111193278858</t>
+  </si>
+  <si>
+    <t>3045987650</t>
+  </si>
+  <si>
+    <t>61962571</t>
+  </si>
+  <si>
+    <t>987388666</t>
+  </si>
+  <si>
+    <t>cliente nit a nit</t>
+  </si>
+  <si>
+    <t>901963208</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -369,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -384,9 +406,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -702,21 +721,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.453125" style="1"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -927,11 +946,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -939,20 +958,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
-    <col min="3" max="3" width="30.1796875" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" customWidth="1"/>
-    <col min="5" max="5" width="21.7265625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
@@ -987,13 +1006,13 @@
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -1027,10 +1046,10 @@
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
@@ -1050,19 +1069,19 @@
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>50</v>
@@ -1073,24 +1092,24 @@
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>23</v>
@@ -1133,28 +1152,28 @@
         <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1">
@@ -1162,28 +1181,28 @@
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1">
@@ -1191,13 +1210,13 @@
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1">
@@ -1205,13 +1224,16 @@
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>69</v>
+      <c r="E12" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1">
@@ -1219,36 +1241,67 @@
         <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>92</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>72</v>
+      <c r="B14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>70</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="1" customFormat="1">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>